<commit_message>
Created a working version for MailProject and added test cases.
</commit_message>
<xml_diff>
--- a/data/test/test_data_source_base.xlsx
+++ b/data/test/test_data_source_base.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
-    <sheet name="project_data" sheetId="2" r:id="rId2"/>
+    <sheet name="project_data_single" sheetId="2" r:id="rId2"/>
+    <sheet name="project_data_multiple" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>client_id</t>
   </si>
@@ -111,6 +112,9 @@
   </si>
   <si>
     <t>Certainly a Project GmbH &amp; Co. KG</t>
+  </si>
+  <si>
+    <t>Another Project GmbH</t>
   </si>
 </sst>
 </file>
@@ -634,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,4 +666,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added translation form column headers to instance attributes.
</commit_message>
<xml_diff>
--- a/data/test/test_data_source_base.xlsx
+++ b/data/test/test_data_source_base.xlsx
@@ -639,7 +639,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more attributes and corresponding tests for MailProject
</commit_message>
<xml_diff>
--- a/data/test/test_data_source_base.xlsx
+++ b/data/test/test_data_source_base.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
-    <sheet name="project_data_single" sheetId="2" r:id="rId2"/>
-    <sheet name="project_data_multiple" sheetId="3" r:id="rId3"/>
+    <sheet name="project_data_single_1" sheetId="2" r:id="rId2"/>
+    <sheet name="project_data_single_2" sheetId="4" r:id="rId3"/>
+    <sheet name="project_data_multiple" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>client_id</t>
   </si>
@@ -115,13 +116,85 @@
   </si>
   <si>
     <t>Another Project GmbH</t>
+  </si>
+  <si>
+    <t>coupon_rate</t>
+  </si>
+  <si>
+    <t>commercial_register_number</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> subscription_am_authorized</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mailing_as_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> depot_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> depot_bic</t>
+  </si>
+  <si>
+    <t>1B3456789</t>
+  </si>
+  <si>
+    <t>123/456789</t>
+  </si>
+  <si>
+    <t>SOMEALPHANUMERICSTRING</t>
+  </si>
+  <si>
+    <t>BIDCDEMXXX</t>
+  </si>
+  <si>
+    <t>ALSOABIC123X</t>
+  </si>
+  <si>
+    <t>00BICNUM120X0</t>
+  </si>
+  <si>
+    <t>0048522358</t>
+  </si>
+  <si>
+    <t>date_issuance</t>
+  </si>
+  <si>
+    <t>date_maturity</t>
+  </si>
+  <si>
+    <t>issue_volume_min</t>
+  </si>
+  <si>
+    <t>issue_volume_max</t>
+  </si>
+  <si>
+    <t>collateral_string</t>
+  </si>
+  <si>
+    <t>HRA 12345 B</t>
+  </si>
+  <si>
+    <t>HRB 04321 A</t>
+  </si>
+  <si>
+    <t>Land Charge and Letter of Comfort</t>
+  </si>
+  <si>
+    <t>Letter of Comfort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +204,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,14 +235,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,9 +568,13 @@
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +602,23 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -540,8 +646,23 @@
       <c r="I2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>50000</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <v>123456789</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -569,8 +690,23 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1000000</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -598,8 +734,23 @@
       <c r="I4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>10000</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -626,6 +777,21 @@
       </c>
       <c r="I5" t="s">
         <v>28</v>
+      </c>
+      <c r="J5">
+        <v>25000</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -636,31 +802,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>141</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43646</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44742</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43830</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44926</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6">
+        <v>4000000</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5000000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -668,38 +965,111 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>141</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="4">
+        <v>43646</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44742</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="H2" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
+      </c>
+      <c r="C3" s="4">
+        <v>43830</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44926</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="6">
+        <v>4000000</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5000000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test for str dunder of MailProject. Added first test and dummy data for the Client class.
</commit_message>
<xml_diff>
--- a/data/test/test_data_source_base.xlsx
+++ b/data/test/test_data_source_base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>80001</v>
       </c>
       <c r="F2" t="s">
@@ -640,7 +640,7 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>80001</v>
       </c>
       <c r="I2" t="s">
@@ -675,7 +675,7 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>80002</v>
       </c>
       <c r="F3" t="s">
@@ -684,7 +684,7 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>80002</v>
       </c>
       <c r="I3" t="s">
@@ -719,7 +719,7 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>80003</v>
       </c>
       <c r="F4" t="s">
@@ -728,7 +728,7 @@
       <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>90003</v>
       </c>
       <c r="I4" t="s">
@@ -763,7 +763,7 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>80004</v>
       </c>
       <c r="F5" t="s">
@@ -772,7 +772,7 @@
       <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>90004</v>
       </c>
       <c r="I5" t="s">
@@ -886,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>